<commit_message>
one rep max algorithm
</commit_message>
<xml_diff>
--- a/doc/plan/dates (version 1).xlsx
+++ b/doc/plan/dates (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1700p\Desktop\Ally\projects\TrainingTracker\TrainingTracker\doc\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7344A3EA-A077-4742-ACE7-069DB1BC1CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B8C83B-240C-4E5E-B8A8-74BA38C4A5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -823,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>

</xml_diff>